<commit_message>
07/09/2019 have done some changed.
</commit_message>
<xml_diff>
--- a/SeleniumKewordAutomation/Data/MyFirstExcel.xlsx
+++ b/SeleniumKewordAutomation/Data/MyFirstExcel.xlsx
@@ -1,13 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="17160" windowHeight="5304"/>
   </bookViews>
   <sheets>
-    <sheet name="Datatypes in Java" r:id="rId3" sheetId="1"/>
+    <sheet name="Datatypes in Java" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -51,10 +54,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -66,7 +68,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -84,18 +86,308 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -106,51 +398,51 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="n">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="n">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="n">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="C4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="n">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -162,6 +454,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>